<commit_message>
Cambios menores en el excel de analisis de riesgos. Creado el archivo de planificacion temporal y de recursos. Borrado el archivo de Informe trabajo integrador (remplazado por primera entrevista)
</commit_message>
<xml_diff>
--- a/Archivos trabajo integrador/Analisis de riesgos.xlsx
+++ b/Archivos trabajo integrador/Analisis de riesgos.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariano Ruarte\Desktop\Trabajo integrador\Archivos trabajo integrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40E0AF7-E099-4004-AC0E-26FBE1D87BB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8535A253-7BB4-40FD-AE3D-7D47137AA63D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="16220" windowHeight="11660" xr2:uid="{F278497A-FD9C-4ED7-99B3-80F2D1AB5CCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Gravedad</t>
   </si>
@@ -82,21 +82,30 @@
     <t>Posibilidad</t>
   </si>
   <si>
-    <t>Corte imprevisto
-de luz</t>
-  </si>
-  <si>
     <t>Día no laboral por
 enfermedad</t>
-  </si>
-  <si>
-    <t>Corrección de errores del
-programa</t>
   </si>
   <si>
     <t>Demora en la obtención
 de recursos
 informáticos</t>
+  </si>
+  <si>
+    <t>Aparición de bugs
+importantes en el 
+programa</t>
+  </si>
+  <si>
+    <t>Averías de computadora</t>
+  </si>
+  <si>
+    <t>Cortes imprevistos
+de luz</t>
+  </si>
+  <si>
+    <t>Retrasos en la creación
+de la documentación
+del proyecto</t>
   </si>
 </sst>
 </file>
@@ -170,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -178,26 +187,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -205,26 +258,64 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -662,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECD2575-0ACB-4556-A03F-2730E1309208}">
   <dimension ref="A2:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28:L28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,497 +764,500 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9" t="s">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="9"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="11">
         <v>5</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4">
+      <c r="D4" s="8"/>
+      <c r="E4" s="13">
         <v>10</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5">
+      <c r="F4" s="14"/>
+      <c r="G4" s="16">
         <v>15</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5">
+      <c r="H4" s="17"/>
+      <c r="I4" s="16">
         <v>20</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5">
+      <c r="J4" s="18"/>
+      <c r="K4" s="18">
         <v>25</v>
       </c>
-      <c r="L4" s="5"/>
+      <c r="L4" s="17"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="1"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="10"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="10"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="1"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="10"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="12"/>
       <c r="L6" s="10"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="1"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="10"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="12"/>
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="1"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="10"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="10"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="12"/>
       <c r="L8" s="10"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="23"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="11">
         <v>4</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4">
+      <c r="D10" s="8"/>
+      <c r="E10" s="13">
         <v>8</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4">
+      <c r="F10" s="14"/>
+      <c r="G10" s="13">
         <v>12</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5">
+      <c r="H10" s="14"/>
+      <c r="I10" s="16">
         <v>16</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5">
+      <c r="J10" s="17"/>
+      <c r="K10" s="18">
         <v>20</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="17"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B11" s="6"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="G11" s="15"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="I11" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="10"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="6"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+      <c r="I12" s="9"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="10"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="6"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="10"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="6"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="12"/>
       <c r="L14" s="10"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="6"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="23"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="11">
         <v>3</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3">
+      <c r="D16" s="8"/>
+      <c r="E16" s="7">
         <v>6</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4">
+      <c r="F16" s="8"/>
+      <c r="G16" s="13">
         <v>9</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4">
+      <c r="H16" s="14"/>
+      <c r="I16" s="13">
         <v>12</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="5">
+      <c r="J16" s="14"/>
+      <c r="K16" s="18">
         <v>15</v>
       </c>
-      <c r="L16" s="5"/>
+      <c r="L16" s="17"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="6"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
       <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B18" s="6"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
       <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
+      <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="6"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="10"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
+      <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="6"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
       <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
+      <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="6"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="23"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="11">
         <v>2</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3">
+      <c r="D22" s="8"/>
+      <c r="E22" s="7">
         <v>4</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3">
+      <c r="F22" s="8"/>
+      <c r="G22" s="7">
         <v>6</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="4">
+      <c r="H22" s="8"/>
+      <c r="I22" s="13">
         <v>8</v>
       </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4">
+      <c r="J22" s="14"/>
+      <c r="K22" s="20">
         <v>10</v>
       </c>
-      <c r="L22" s="4"/>
+      <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B23" s="6"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="10"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="6"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="10"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B25" s="6"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="10"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="6"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="10"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="6"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="23"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="11">
         <v>1</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3">
+      <c r="D28" s="8"/>
+      <c r="E28" s="7">
         <v>2</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3">
+      <c r="F28" s="8"/>
+      <c r="G28" s="7">
         <v>3</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3">
+      <c r="H28" s="8"/>
+      <c r="I28" s="7">
         <v>4</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3">
+      <c r="J28" s="8"/>
+      <c r="K28" s="11">
         <v>5</v>
       </c>
-      <c r="L28" s="3"/>
+      <c r="L28" s="8"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="6"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="10"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B30" s="6"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="10"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B31" s="6"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="10"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="10"/>
     </row>
     <row r="33" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="7"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="I29:J33"/>
     <mergeCell ref="K29:L33"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="K23:L27"/>
@@ -1176,16 +1270,17 @@
     <mergeCell ref="C29:D33"/>
     <mergeCell ref="E29:F33"/>
     <mergeCell ref="G29:H33"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="B22:B27"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I29:J33"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="C23:D27"/>
     <mergeCell ref="E23:F27"/>
     <mergeCell ref="G23:H27"/>
     <mergeCell ref="I23:J27"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="C17:D21"/>
     <mergeCell ref="E17:F21"/>
@@ -1198,32 +1293,32 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
+    <mergeCell ref="G5:H9"/>
+    <mergeCell ref="I5:J9"/>
+    <mergeCell ref="K5:L9"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C11:D15"/>
+    <mergeCell ref="E11:F15"/>
+    <mergeCell ref="G11:H15"/>
+    <mergeCell ref="I11:J15"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="K10:L10"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="C11:D15"/>
-    <mergeCell ref="E11:F15"/>
-    <mergeCell ref="G11:H15"/>
-    <mergeCell ref="I11:J15"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="G5:H9"/>
-    <mergeCell ref="I5:J9"/>
-    <mergeCell ref="K5:L9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C5:D9"/>
     <mergeCell ref="E5:F9"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>